<commit_message>
Added the rest of files
</commit_message>
<xml_diff>
--- a/Synthesis/Tongali/Trial synthesis 2 (tongali)/Modal Distribution Program Parameter Changes.xlsx
+++ b/Synthesis/Tongali/Trial synthesis 2 (tongali)/Modal Distribution Program Parameter Changes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianbagaforo/Desktop/ECE198/Synthesis/Trial synthesis 2 (tongali)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianbagaforo/Desktop/ECE198/Synthesis/Tongali/Trial synthesis 2 (tongali)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12893832-1BC9-6F4F-806F-B93F7B671467}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F2018A-ED97-2447-BAFB-F5AC1D93B7D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="11380" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14780" yWindow="460" windowWidth="11380" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="158" sheetId="3" r:id="rId1"/>
@@ -425,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I31" zoomScale="91" workbookViewId="0">
-      <selection activeCell="O62" sqref="O62"/>
+    <sheetView tabSelected="1" topLeftCell="G42" zoomScale="91" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2242,6 +2242,78 @@
       </c>
       <c r="N63" s="9" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G65">
+        <f>G40/F40</f>
+        <v>822.5</v>
+      </c>
+    </row>
+    <row r="66" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G66">
+        <f t="shared" ref="G66:G80" si="0">G41/F41</f>
+        <v>892.6010362694301</v>
+      </c>
+    </row>
+    <row r="67" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G67">
+        <f t="shared" si="0"/>
+        <v>1163.8857142857144</v>
+      </c>
+    </row>
+    <row r="68" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G68">
+        <f t="shared" si="0"/>
+        <v>1040.3815789473686</v>
+      </c>
+    </row>
+    <row r="69" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G69">
+        <f t="shared" si="0"/>
+        <v>1168.4104477611941</v>
+      </c>
+    </row>
+    <row r="70" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G70">
+        <f t="shared" si="0"/>
+        <v>1742.3362068965519</v>
+      </c>
+    </row>
+    <row r="71" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G71">
+        <f t="shared" si="0"/>
+        <v>1661.7346938775511</v>
+      </c>
+    </row>
+    <row r="72" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G72">
+        <f t="shared" si="0"/>
+        <v>1832.1428571428571</v>
+      </c>
+    </row>
+    <row r="73" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G73">
+        <f t="shared" si="0"/>
+        <v>2171.3333333333335</v>
+      </c>
+    </row>
+    <row r="74" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G74">
+        <f t="shared" si="0"/>
+        <v>2185.0757575757575</v>
+      </c>
+    </row>
+    <row r="75" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G75">
+        <f>G50/F50</f>
+        <v>2664.1578947368421</v>
+      </c>
+    </row>
+    <row r="76" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G76">
+        <f t="shared" si="0"/>
+        <v>3041.1153846153848</v>
       </c>
     </row>
   </sheetData>

</xml_diff>